<commit_message>
Swing branch was created
</commit_message>
<xml_diff>
--- a/Java hint.xlsx
+++ b/Java hint.xlsx
@@ -18,6 +18,7 @@
     <sheet name="Regex" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -8469,36 +8470,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -8534,6 +8505,36 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9202,12 +9203,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
@@ -9268,20 +9269,20 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="74" t="s">
+      <c r="A7" s="64" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
+      <c r="B7" s="64"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
     </row>
     <row r="8" spans="1:7" s="31" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="75" t="s">
+      <c r="A8" s="65" t="s">
         <v>85</v>
       </c>
-      <c r="B8" s="75"/>
-      <c r="C8" s="75"/>
-      <c r="D8" s="75"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="65"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C9" s="35"/>
@@ -9293,26 +9294,26 @@
       <c r="B10" s="52"/>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="65" t="s">
+      <c r="A11" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="B11" s="65"/>
+      <c r="B11" s="55"/>
     </row>
     <row r="12" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="65" t="s">
+      <c r="A12" s="55" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="65"/>
+      <c r="B12" s="55"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="73" t="s">
+      <c r="A14" s="63" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="73"/>
-      <c r="C14" s="73" t="s">
+      <c r="B14" s="63"/>
+      <c r="C14" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="73"/>
+      <c r="D14" s="63"/>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
@@ -9396,21 +9397,21 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="67" t="s">
+      <c r="A20" s="57" t="s">
         <v>80</v>
       </c>
-      <c r="B20" s="68"/>
-      <c r="C20" s="68"/>
-      <c r="D20" s="69"/>
+      <c r="B20" s="58"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="59"/>
       <c r="E20" s="29"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="70" t="s">
+      <c r="A21" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="71"/>
-      <c r="C21" s="71"/>
-      <c r="D21" s="72"/>
+      <c r="B21" s="61"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="62"/>
     </row>
     <row r="22" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="30"/>
@@ -9419,12 +9420,12 @@
       <c r="D22" s="30"/>
     </row>
     <row r="23" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="60" t="s">
+      <c r="A23" s="72" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="60"/>
-      <c r="C23" s="60"/>
-      <c r="D23" s="60"/>
+      <c r="B23" s="72"/>
+      <c r="C23" s="72"/>
+      <c r="D23" s="72"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
@@ -9433,20 +9434,20 @@
       <c r="D24" s="15"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="57" t="s">
+      <c r="A25" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="58"/>
-      <c r="C25" s="58"/>
-      <c r="D25" s="59"/>
+      <c r="B25" s="67"/>
+      <c r="C25" s="67"/>
+      <c r="D25" s="68"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="57" t="s">
+      <c r="A26" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="58"/>
-      <c r="C26" s="58"/>
-      <c r="D26" s="59"/>
+      <c r="B26" s="67"/>
+      <c r="C26" s="67"/>
+      <c r="D26" s="68"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="21"/>
@@ -9455,28 +9456,28 @@
       <c r="D27" s="23"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="57" t="s">
+      <c r="A28" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="58"/>
-      <c r="C28" s="58"/>
-      <c r="D28" s="59"/>
+      <c r="B28" s="67"/>
+      <c r="C28" s="67"/>
+      <c r="D28" s="68"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="57" t="s">
+      <c r="A29" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="B29" s="58"/>
-      <c r="C29" s="58"/>
-      <c r="D29" s="59"/>
+      <c r="B29" s="67"/>
+      <c r="C29" s="67"/>
+      <c r="D29" s="68"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="57" t="s">
+      <c r="A30" s="66" t="s">
         <v>266</v>
       </c>
-      <c r="B30" s="58"/>
-      <c r="C30" s="58"/>
-      <c r="D30" s="59"/>
+      <c r="B30" s="67"/>
+      <c r="C30" s="67"/>
+      <c r="D30" s="68"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="32"/>
@@ -9485,44 +9486,44 @@
       <c r="D31" s="34"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="57" t="s">
+      <c r="A32" s="66" t="s">
         <v>82</v>
       </c>
-      <c r="B32" s="58"/>
-      <c r="C32" s="58"/>
-      <c r="D32" s="59"/>
+      <c r="B32" s="67"/>
+      <c r="C32" s="67"/>
+      <c r="D32" s="68"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="66" t="s">
+      <c r="A33" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="B33" s="66"/>
-      <c r="C33" s="66"/>
-      <c r="D33" s="66"/>
+      <c r="B33" s="56"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="56"/>
     </row>
     <row r="34" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="61" t="s">
+      <c r="A34" s="73" t="s">
         <v>89</v>
       </c>
-      <c r="B34" s="62"/>
-      <c r="C34" s="62"/>
-      <c r="D34" s="63"/>
+      <c r="B34" s="74"/>
+      <c r="C34" s="74"/>
+      <c r="D34" s="75"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="57" t="s">
+      <c r="A35" s="66" t="s">
         <v>83</v>
       </c>
-      <c r="B35" s="58"/>
-      <c r="C35" s="58"/>
-      <c r="D35" s="59"/>
+      <c r="B35" s="67"/>
+      <c r="C35" s="67"/>
+      <c r="D35" s="68"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="57" t="s">
+      <c r="A36" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="B36" s="58"/>
-      <c r="C36" s="58"/>
-      <c r="D36" s="59"/>
+      <c r="B36" s="67"/>
+      <c r="C36" s="67"/>
+      <c r="D36" s="68"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="36"/>
@@ -9531,20 +9532,20 @@
       <c r="D37" s="38"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="57" t="s">
+      <c r="A38" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="B38" s="58"/>
-      <c r="C38" s="58"/>
-      <c r="D38" s="59"/>
+      <c r="B38" s="67"/>
+      <c r="C38" s="67"/>
+      <c r="D38" s="68"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="54" t="s">
+      <c r="A39" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="B39" s="55"/>
-      <c r="C39" s="55"/>
-      <c r="D39" s="56"/>
+      <c r="B39" s="70"/>
+      <c r="C39" s="70"/>
+      <c r="D39" s="71"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="24"/>
@@ -9560,6 +9561,16 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A34:D34"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -9573,16 +9584,6 @@
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="A29:D29"/>
     <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A39:D39"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A34:D34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Java hint.xlsx updated (Android DB).
</commit_message>
<xml_diff>
--- a/Java hint.xlsx
+++ b/Java hint.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="289">
   <si>
     <t>Структура пакетов</t>
   </si>
@@ -8084,13 +8084,61 @@
   </si>
   <si>
     <t>Асинхронность и организация многопоточности</t>
+  </si>
+  <si>
+    <t>Работа с SQLite</t>
+  </si>
+  <si>
+    <t>1 helper class = you don't need to synchronize and you can use the helper from multiple readers/writers because helper class manages synchronization itself</t>
+  </si>
+  <si>
+    <t>SqliteOpenHelper object holds on to one database connection</t>
+  </si>
+  <si>
+    <t>NOT be doing db accesses from the UI thread</t>
+  </si>
+  <si>
+    <t>Call the read-only, and you'll get the write database connection regardless.</t>
+  </si>
+  <si>
+    <t>So, one helper instance, one db connection.</t>
+  </si>
+  <si>
+    <t> The SqliteDatabase object uses java locks to keep access serialized.</t>
+  </si>
+  <si>
+    <t>So, multiple threads? Use one helper.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQLite implements a exclusive write lock, shared read lock model. This means that you can have concurrent readers active in the database at the same time or a single writer, you can't have both. If you use the WAL logging feature you can have a single writer and multiple readers active in the database at the same time, but you still can't have more than one writer. </t>
+  </si>
+  <si>
+    <t>If you try to write to the database from actual distinct connections at the same time, one will fail. Worse, if you don’t call the right version of insert/update on the SQLiteDatabase, you won’t get an exception. You’ll just get a message in your LogCat, and that will be it. Period.</t>
+  </si>
+  <si>
+    <t>Use a singleton helper for opening connections. 1) Open as many readable connections as you want, and close then after your are done with it. 2) For writable connections, you should open only a single writable connection.</t>
+  </si>
+  <si>
+    <t>If you are going to perform more than one update of any kind, wrap it in a transaction.  It seems like the 50 updates I do in the transaction (this was in the original app version, not the new one) take the same amount of time as the 1 update outside of the transaction.</t>
+  </si>
+  <si>
+    <t>sqlite database should be opened only once. Close it in onDestroy()</t>
+  </si>
+  <si>
+    <t>https://enterra.ru/blog/android_issues_with_sqlite/</t>
+  </si>
+  <si>
+    <t>https://touchlabblog.tumblr.com/post/24474398246/android-sqlite-locking</t>
+  </si>
+  <si>
+    <t>https://touchlabblog.tumblr.com/post/24474750219/single-sqlite-connection</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -8210,8 +8258,17 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -8257,6 +8314,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF7171"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8362,10 +8425,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -8471,6 +8535,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -8554,8 +8621,14 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -8879,7 +8952,7 @@
       <c r="A1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="49" t="s">
         <v>5</v>
       </c>
     </row>
@@ -8887,21 +8960,21 @@
       <c r="A2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="48"/>
+      <c r="B2" s="49"/>
     </row>
     <row r="3" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
     </row>
     <row r="4" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="50" t="s">
         <v>188</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -8909,11 +8982,11 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="49" t="s">
+      <c r="A7" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="49"/>
-      <c r="C7" s="49"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -8928,11 +9001,11 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="50" t="s">
+      <c r="A10" s="51" t="s">
         <v>254</v>
       </c>
-      <c r="B10" s="50"/>
-      <c r="C10" s="50"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -8999,19 +9072,19 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38" customWidth="1"/>
+    <col min="1" max="1" width="150.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="77" t="s">
         <v>272</v>
       </c>
     </row>
@@ -9040,8 +9113,94 @@
         <v>271</v>
       </c>
     </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="77" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="48" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="39" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="39" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="39" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="78" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="79" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="78" t="s">
+        <v>288</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A25" r:id="rId1"/>
+    <hyperlink ref="A26" r:id="rId2"/>
+    <hyperlink ref="A27" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -9124,10 +9283,10 @@
       <c r="C4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="51" t="s">
+      <c r="D4" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="E4" s="51"/>
+      <c r="E4" s="52"/>
       <c r="F4" s="7" t="s">
         <v>31</v>
       </c>
@@ -9186,14 +9345,14 @@
       <c r="A9" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="53" t="s">
+      <c r="C9" s="52"/>
+      <c r="D9" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="53"/>
+      <c r="E9" s="54"/>
       <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9215,22 +9374,22 @@
       <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="52" t="s">
+      <c r="A11" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="52"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="48" t="s">
+      <c r="A12" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="48"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
@@ -9269,12 +9428,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="65" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
@@ -9335,51 +9494,51 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="74" t="s">
+      <c r="A7" s="75" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
     </row>
     <row r="8" spans="1:7" s="31" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="75" t="s">
+      <c r="A8" s="76" t="s">
         <v>85</v>
       </c>
-      <c r="B8" s="75"/>
-      <c r="C8" s="75"/>
-      <c r="D8" s="75"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="76"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C9" s="35"/>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="52"/>
+      <c r="B10" s="53"/>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="65" t="s">
+      <c r="A11" s="66" t="s">
         <v>77</v>
       </c>
-      <c r="B11" s="65"/>
+      <c r="B11" s="66"/>
     </row>
     <row r="12" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="65" t="s">
+      <c r="A12" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="65"/>
+      <c r="B12" s="66"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="73" t="s">
+      <c r="A14" s="74" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="73"/>
-      <c r="C14" s="73" t="s">
+      <c r="B14" s="74"/>
+      <c r="C14" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="73"/>
+      <c r="D14" s="74"/>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
@@ -9463,21 +9622,21 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="67" t="s">
+      <c r="A20" s="68" t="s">
         <v>80</v>
       </c>
-      <c r="B20" s="68"/>
-      <c r="C20" s="68"/>
-      <c r="D20" s="69"/>
+      <c r="B20" s="69"/>
+      <c r="C20" s="69"/>
+      <c r="D20" s="70"/>
       <c r="E20" s="29"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="70" t="s">
+      <c r="A21" s="71" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="71"/>
-      <c r="C21" s="71"/>
-      <c r="D21" s="72"/>
+      <c r="B21" s="72"/>
+      <c r="C21" s="72"/>
+      <c r="D21" s="73"/>
     </row>
     <row r="22" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="30"/>
@@ -9486,12 +9645,12 @@
       <c r="D22" s="30"/>
     </row>
     <row r="23" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="60" t="s">
+      <c r="A23" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="60"/>
-      <c r="C23" s="60"/>
-      <c r="D23" s="60"/>
+      <c r="B23" s="61"/>
+      <c r="C23" s="61"/>
+      <c r="D23" s="61"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
@@ -9500,20 +9659,20 @@
       <c r="D24" s="15"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="57" t="s">
+      <c r="A25" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="58"/>
-      <c r="C25" s="58"/>
-      <c r="D25" s="59"/>
+      <c r="B25" s="59"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="60"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="57" t="s">
+      <c r="A26" s="58" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="58"/>
-      <c r="C26" s="58"/>
-      <c r="D26" s="59"/>
+      <c r="B26" s="59"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="60"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="21"/>
@@ -9522,28 +9681,28 @@
       <c r="D27" s="23"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="57" t="s">
+      <c r="A28" s="58" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="58"/>
-      <c r="C28" s="58"/>
-      <c r="D28" s="59"/>
+      <c r="B28" s="59"/>
+      <c r="C28" s="59"/>
+      <c r="D28" s="60"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="57" t="s">
+      <c r="A29" s="58" t="s">
         <v>88</v>
       </c>
-      <c r="B29" s="58"/>
-      <c r="C29" s="58"/>
-      <c r="D29" s="59"/>
+      <c r="B29" s="59"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="60"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="57" t="s">
+      <c r="A30" s="58" t="s">
         <v>266</v>
       </c>
-      <c r="B30" s="58"/>
-      <c r="C30" s="58"/>
-      <c r="D30" s="59"/>
+      <c r="B30" s="59"/>
+      <c r="C30" s="59"/>
+      <c r="D30" s="60"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="32"/>
@@ -9552,44 +9711,44 @@
       <c r="D31" s="34"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="57" t="s">
+      <c r="A32" s="58" t="s">
         <v>82</v>
       </c>
-      <c r="B32" s="58"/>
-      <c r="C32" s="58"/>
-      <c r="D32" s="59"/>
+      <c r="B32" s="59"/>
+      <c r="C32" s="59"/>
+      <c r="D32" s="60"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="66" t="s">
+      <c r="A33" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="B33" s="66"/>
-      <c r="C33" s="66"/>
-      <c r="D33" s="66"/>
+      <c r="B33" s="67"/>
+      <c r="C33" s="67"/>
+      <c r="D33" s="67"/>
     </row>
     <row r="34" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="61" t="s">
+      <c r="A34" s="62" t="s">
         <v>89</v>
       </c>
-      <c r="B34" s="62"/>
-      <c r="C34" s="62"/>
-      <c r="D34" s="63"/>
+      <c r="B34" s="63"/>
+      <c r="C34" s="63"/>
+      <c r="D34" s="64"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="57" t="s">
+      <c r="A35" s="58" t="s">
         <v>83</v>
       </c>
-      <c r="B35" s="58"/>
-      <c r="C35" s="58"/>
-      <c r="D35" s="59"/>
+      <c r="B35" s="59"/>
+      <c r="C35" s="59"/>
+      <c r="D35" s="60"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="57" t="s">
+      <c r="A36" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="B36" s="58"/>
-      <c r="C36" s="58"/>
-      <c r="D36" s="59"/>
+      <c r="B36" s="59"/>
+      <c r="C36" s="59"/>
+      <c r="D36" s="60"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="36"/>
@@ -9598,20 +9757,20 @@
       <c r="D37" s="38"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="57" t="s">
+      <c r="A38" s="58" t="s">
         <v>61</v>
       </c>
-      <c r="B38" s="58"/>
-      <c r="C38" s="58"/>
-      <c r="D38" s="59"/>
+      <c r="B38" s="59"/>
+      <c r="C38" s="59"/>
+      <c r="D38" s="60"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="54" t="s">
+      <c r="A39" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="B39" s="55"/>
-      <c r="C39" s="55"/>
-      <c r="D39" s="56"/>
+      <c r="B39" s="56"/>
+      <c r="C39" s="56"/>
+      <c r="D39" s="57"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="24"/>

</xml_diff>

<commit_message>
Java hint.xlsx updated 2 (Android DB).
</commit_message>
<xml_diff>
--- a/Java hint.xlsx
+++ b/Java hint.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="290">
   <si>
     <t>Структура пакетов</t>
   </si>
@@ -8132,6 +8132,9 @@
   </si>
   <si>
     <t>https://touchlabblog.tumblr.com/post/24474750219/single-sqlite-connection</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/2493331/what-are-the-best-practices-for-sqlite-on-android#comment80343236_2493331</t>
   </si>
 </sst>
 </file>
@@ -8537,6 +8540,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -8554,36 +8562,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -8621,9 +8599,34 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -8952,7 +8955,7 @@
       <c r="A1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="52" t="s">
         <v>5</v>
       </c>
     </row>
@@ -8960,21 +8963,21 @@
       <c r="A2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="49"/>
+      <c r="B2" s="52"/>
     </row>
     <row r="3" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
     </row>
     <row r="4" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="53" t="s">
         <v>188</v>
       </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -8982,11 +8985,11 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="50" t="s">
+      <c r="A7" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -9001,11 +9004,11 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="54" t="s">
         <v>254</v>
       </c>
-      <c r="B10" s="51"/>
-      <c r="C10" s="51"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="54"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -9072,10 +9075,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A27"/>
+  <dimension ref="A1:A28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9084,7 +9087,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="49" t="s">
         <v>272</v>
       </c>
     </row>
@@ -9114,7 +9117,7 @@
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="77" t="s">
+      <c r="A10" s="49" t="s">
         <v>273</v>
       </c>
     </row>
@@ -9179,28 +9182,34 @@
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="78" t="s">
+      <c r="A25" s="50" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="79" t="s">
+      <c r="A26" s="50" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="51" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="78" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="50" t="s">
         <v>288</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A25" r:id="rId1"/>
-    <hyperlink ref="A26" r:id="rId2"/>
-    <hyperlink ref="A27" r:id="rId3"/>
+    <hyperlink ref="A27" r:id="rId1"/>
+    <hyperlink ref="A28" r:id="rId2"/>
+    <hyperlink ref="A25" r:id="rId3"/>
+    <hyperlink ref="A26" r:id="rId4" location="comment80343236_2493331"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -9283,10 +9292,10 @@
       <c r="C4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="52" t="s">
+      <c r="D4" s="55" t="s">
         <v>69</v>
       </c>
-      <c r="E4" s="52"/>
+      <c r="E4" s="55"/>
       <c r="F4" s="7" t="s">
         <v>31</v>
       </c>
@@ -9345,14 +9354,14 @@
       <c r="A9" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="52"/>
-      <c r="D9" s="54" t="s">
+      <c r="C9" s="55"/>
+      <c r="D9" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="54"/>
+      <c r="E9" s="57"/>
       <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9374,22 +9383,22 @@
       <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="53" t="s">
+      <c r="A11" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="53"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="49" t="s">
+      <c r="A12" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="49"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
@@ -9428,12 +9437,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
@@ -9494,51 +9503,51 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="68" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="75"/>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
+      <c r="B7" s="68"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
     </row>
     <row r="8" spans="1:7" s="31" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="76" t="s">
+      <c r="A8" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="B8" s="76"/>
-      <c r="C8" s="76"/>
-      <c r="D8" s="76"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="69"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C9" s="35"/>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="53" t="s">
+      <c r="A10" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="53"/>
+      <c r="B10" s="56"/>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="66" t="s">
+      <c r="A11" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="B11" s="66"/>
+      <c r="B11" s="59"/>
     </row>
     <row r="12" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="66" t="s">
+      <c r="A12" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="66"/>
+      <c r="B12" s="59"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="74" t="s">
+      <c r="A14" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="74"/>
-      <c r="C14" s="74" t="s">
+      <c r="B14" s="67"/>
+      <c r="C14" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="74"/>
+      <c r="D14" s="67"/>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
@@ -9622,21 +9631,21 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="68" t="s">
+      <c r="A20" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="B20" s="69"/>
-      <c r="C20" s="69"/>
-      <c r="D20" s="70"/>
+      <c r="B20" s="62"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="63"/>
       <c r="E20" s="29"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="71" t="s">
+      <c r="A21" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="72"/>
-      <c r="C21" s="72"/>
-      <c r="D21" s="73"/>
+      <c r="B21" s="65"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="66"/>
     </row>
     <row r="22" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="30"/>
@@ -9645,12 +9654,12 @@
       <c r="D22" s="30"/>
     </row>
     <row r="23" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="61" t="s">
+      <c r="A23" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="61"/>
-      <c r="C23" s="61"/>
-      <c r="D23" s="61"/>
+      <c r="B23" s="76"/>
+      <c r="C23" s="76"/>
+      <c r="D23" s="76"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
@@ -9659,20 +9668,20 @@
       <c r="D24" s="15"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="58" t="s">
+      <c r="A25" s="70" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="59"/>
-      <c r="C25" s="59"/>
-      <c r="D25" s="60"/>
+      <c r="B25" s="71"/>
+      <c r="C25" s="71"/>
+      <c r="D25" s="72"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="58" t="s">
+      <c r="A26" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="59"/>
-      <c r="C26" s="59"/>
-      <c r="D26" s="60"/>
+      <c r="B26" s="71"/>
+      <c r="C26" s="71"/>
+      <c r="D26" s="72"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="21"/>
@@ -9681,28 +9690,28 @@
       <c r="D27" s="23"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="58" t="s">
+      <c r="A28" s="70" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="59"/>
-      <c r="C28" s="59"/>
-      <c r="D28" s="60"/>
+      <c r="B28" s="71"/>
+      <c r="C28" s="71"/>
+      <c r="D28" s="72"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="58" t="s">
+      <c r="A29" s="70" t="s">
         <v>88</v>
       </c>
-      <c r="B29" s="59"/>
-      <c r="C29" s="59"/>
-      <c r="D29" s="60"/>
+      <c r="B29" s="71"/>
+      <c r="C29" s="71"/>
+      <c r="D29" s="72"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="58" t="s">
+      <c r="A30" s="70" t="s">
         <v>266</v>
       </c>
-      <c r="B30" s="59"/>
-      <c r="C30" s="59"/>
-      <c r="D30" s="60"/>
+      <c r="B30" s="71"/>
+      <c r="C30" s="71"/>
+      <c r="D30" s="72"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="32"/>
@@ -9711,44 +9720,44 @@
       <c r="D31" s="34"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="58" t="s">
+      <c r="A32" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="B32" s="59"/>
-      <c r="C32" s="59"/>
-      <c r="D32" s="60"/>
+      <c r="B32" s="71"/>
+      <c r="C32" s="71"/>
+      <c r="D32" s="72"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="67" t="s">
+      <c r="A33" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="B33" s="67"/>
-      <c r="C33" s="67"/>
-      <c r="D33" s="67"/>
+      <c r="B33" s="60"/>
+      <c r="C33" s="60"/>
+      <c r="D33" s="60"/>
     </row>
     <row r="34" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="62" t="s">
+      <c r="A34" s="77" t="s">
         <v>89</v>
       </c>
-      <c r="B34" s="63"/>
-      <c r="C34" s="63"/>
-      <c r="D34" s="64"/>
+      <c r="B34" s="78"/>
+      <c r="C34" s="78"/>
+      <c r="D34" s="79"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="58" t="s">
+      <c r="A35" s="70" t="s">
         <v>83</v>
       </c>
-      <c r="B35" s="59"/>
-      <c r="C35" s="59"/>
-      <c r="D35" s="60"/>
+      <c r="B35" s="71"/>
+      <c r="C35" s="71"/>
+      <c r="D35" s="72"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="58" t="s">
+      <c r="A36" s="70" t="s">
         <v>87</v>
       </c>
-      <c r="B36" s="59"/>
-      <c r="C36" s="59"/>
-      <c r="D36" s="60"/>
+      <c r="B36" s="71"/>
+      <c r="C36" s="71"/>
+      <c r="D36" s="72"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="36"/>
@@ -9757,20 +9766,20 @@
       <c r="D37" s="38"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="58" t="s">
+      <c r="A38" s="70" t="s">
         <v>61</v>
       </c>
-      <c r="B38" s="59"/>
-      <c r="C38" s="59"/>
-      <c r="D38" s="60"/>
+      <c r="B38" s="71"/>
+      <c r="C38" s="71"/>
+      <c r="D38" s="72"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="55" t="s">
+      <c r="A39" s="73" t="s">
         <v>60</v>
       </c>
-      <c r="B39" s="56"/>
-      <c r="C39" s="56"/>
-      <c r="D39" s="57"/>
+      <c r="B39" s="74"/>
+      <c r="C39" s="74"/>
+      <c r="D39" s="75"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="24"/>
@@ -9786,6 +9795,16 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A34:D34"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -9799,16 +9818,6 @@
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="A29:D29"/>
     <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A39:D39"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A34:D34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>